<commit_message>
sol145 modified with new information. couple system.
</commit_message>
<xml_diff>
--- a/datFiles_numbering/red.freq.xlsx
+++ b/datFiles_numbering/red.freq.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuhoo\PycharmProjects\stripTheory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuhoo\PycharmProjects\stripTheory\datFiles_numbering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EE5E897-D31B-428B-B016-8C26B4AE80B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02DF247-E577-45D2-88AA-5D5282D6903E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$10</definedName>
@@ -52,9 +54,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -86,10 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -403,31 +406,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:19">
       <c r="A1">
         <v>52000</v>
       </c>
       <c r="B1">
         <v>239300</v>
+      </c>
+      <c r="C1" s="1">
+        <v>4.2002480000000002</v>
       </c>
       <c r="D1">
         <f>(B1-A1)/19</f>
         <v>9857.894736842105</v>
       </c>
       <c r="F1" s="2">
-        <f>2*PI()*O$1*L1/P$1</f>
+        <f t="shared" ref="F1:F10" si="0">2*PI()*O$1*L1/P$1</f>
         <v>0.5220070353204801</v>
       </c>
       <c r="H1">
@@ -457,14 +463,23 @@
       <c r="P1" s="1">
         <v>127600</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1"/>
+      <c r="S1" s="3">
+        <f>2*PI()*O$1*C1/P$1</f>
+        <v>0.41365104263495989</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <f>A1+D$1</f>
         <v>61857.894736842107</v>
       </c>
+      <c r="C2" s="1">
+        <f>C1+J$17</f>
+        <v>8.756056714285716</v>
+      </c>
       <c r="F2" s="2">
-        <f>2*PI()*O$1*L2/P$1</f>
+        <f t="shared" si="0"/>
         <v>0.92213169965496167</v>
       </c>
       <c r="H2">
@@ -488,14 +503,22 @@
       <c r="N2" s="1">
         <v>3461.2040000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="S2" s="3">
+        <f t="shared" ref="S2:S15" si="1">2*PI()*O$1*C2/P$1</f>
+        <v>0.86231860338606858</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
-        <f t="shared" ref="A3:A20" si="0">A2+D$1</f>
+        <f t="shared" ref="A3:A20" si="2">A2+D$1</f>
         <v>71715.789473684214</v>
       </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C20" si="3">C2+J$17</f>
+        <v>13.31186542857143</v>
+      </c>
       <c r="F3" s="2">
-        <f>2*PI()*O$1*L3/P$1</f>
+        <f t="shared" si="0"/>
         <v>1.1832971225917692</v>
       </c>
       <c r="H3">
@@ -519,14 +542,22 @@
       <c r="N3" s="1">
         <v>5699.402</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="S3" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3109861641371769</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
+        <f t="shared" si="2"/>
+        <v>81573.68421052632</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="3"/>
+        <v>17.867674142857144</v>
+      </c>
+      <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>81573.68421052632</v>
-      </c>
-      <c r="F4" s="2">
-        <f>2*PI()*O$1*L4/P$1</f>
         <v>1.3115253137729621</v>
       </c>
       <c r="H4">
@@ -550,14 +581,22 @@
       <c r="N4" s="1">
         <v>7001.5550000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="S4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7596537248882853</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
+        <f t="shared" si="2"/>
+        <v>91431.578947368427</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="3"/>
+        <v>22.423482857142858</v>
+      </c>
+      <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>91431.578947368427</v>
-      </c>
-      <c r="F5" s="2">
-        <f>2*PI()*O$1*L5/P$1</f>
         <v>2.8118150440636414</v>
       </c>
       <c r="H5">
@@ -581,14 +620,22 @@
       <c r="N5" s="1">
         <v>32182.13</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="S5" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2083212856393937</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
+        <f t="shared" si="2"/>
+        <v>101289.47368421053</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="3"/>
+        <v>26.979291571428572</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>101289.47368421053</v>
-      </c>
-      <c r="F6" s="2">
-        <f>2*PI()*O$1*L6/P$1</f>
         <v>3.2412097006418041</v>
       </c>
       <c r="H6">
@@ -612,14 +659,22 @@
       <c r="N6" s="1">
         <v>42761.78</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="S6" s="3">
+        <f t="shared" si="1"/>
+        <v>2.6569888463905023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
+        <f t="shared" si="2"/>
+        <v>111147.36842105264</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="3"/>
+        <v>31.535100285714286</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>111147.36842105264</v>
-      </c>
-      <c r="F7" s="2">
-        <f>2*PI()*O$1*L7/P$1</f>
         <v>3.6741635157936572</v>
       </c>
       <c r="H7">
@@ -643,14 +698,22 @@
       <c r="N7" s="1">
         <v>54948.81</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="S7" s="3">
+        <f t="shared" si="1"/>
+        <v>3.1056564071416108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
+        <f t="shared" si="2"/>
+        <v>121005.26315789475</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="3"/>
+        <v>36.090909000000003</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>121005.26315789475</v>
-      </c>
-      <c r="F8" s="2">
-        <f>2*PI()*O$1*L8/P$1</f>
         <v>6.8216454245773273</v>
       </c>
       <c r="H8">
@@ -674,14 +737,22 @@
       <c r="N8" s="1">
         <v>189417.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="S8" s="3">
+        <f t="shared" si="1"/>
+        <v>3.5543239678927194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
+        <f t="shared" si="2"/>
+        <v>130863.15789473685</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="3"/>
+        <v>40.646717714285721</v>
+      </c>
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>130863.15789473685</v>
-      </c>
-      <c r="F9" s="2">
-        <f>2*PI()*O$1*L9/P$1</f>
         <v>7.6720568290489854</v>
       </c>
       <c r="H9">
@@ -705,14 +776,22 @@
       <c r="N9" s="1">
         <v>239587.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="S9" s="3">
+        <f t="shared" si="1"/>
+        <v>4.002991528643828</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
+        <f t="shared" si="2"/>
+        <v>140721.05263157896</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="3"/>
+        <v>45.202526428571439</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>140721.05263157896</v>
-      </c>
-      <c r="F10" s="2">
-        <f>2*PI()*O$1*L10/P$1</f>
         <v>10.956673688875624</v>
       </c>
       <c r="H10">
@@ -736,11 +815,19 @@
       <c r="N10" s="1">
         <v>488651.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="S10" s="3">
+        <f t="shared" si="1"/>
+        <v>4.451659089394937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>150578.94736842107</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="3"/>
+        <v>49.758335142857156</v>
       </c>
       <c r="F11" s="1"/>
       <c r="L11" t="s">
@@ -752,67 +839,418 @@
       <c r="P11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="S11" s="3">
+        <f t="shared" si="1"/>
+        <v>4.9003266501460452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>160436.84210526317</v>
       </c>
+      <c r="C12" s="1">
+        <f t="shared" si="3"/>
+        <v>54.314143857142874</v>
+      </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="S12" s="3">
+        <f t="shared" si="1"/>
+        <v>5.3489942108971551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>170294.73684210528</v>
       </c>
+      <c r="C13" s="1">
+        <f t="shared" si="3"/>
+        <v>58.869952571428591</v>
+      </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="S13" s="3">
+        <f t="shared" si="1"/>
+        <v>5.7976617716482632</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>180152.63157894739</v>
       </c>
+      <c r="C14" s="1">
+        <f t="shared" si="3"/>
+        <v>63.425761285714309</v>
+      </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="S14" s="3">
+        <f t="shared" si="1"/>
+        <v>6.2463293323993714</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>190010.5263157895</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="C15" s="1">
+        <f t="shared" si="3"/>
+        <v>67.981570000000019</v>
+      </c>
+      <c r="S15" s="3">
+        <f t="shared" si="1"/>
+        <v>6.6949968931504804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>199868.4210526316</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="C16" s="1"/>
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>209726.31578947371</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="C17" s="1"/>
+      <c r="H17" s="1">
+        <v>4.2002480000000002</v>
+      </c>
+      <c r="J17" s="1">
+        <f>(H26-H17)/14</f>
+        <v>4.5558087142857149</v>
+      </c>
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>219584.21052631582</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C18" s="1"/>
+      <c r="H18" s="1">
+        <v>8.0901399999999999</v>
+      </c>
+      <c r="S18" s="3"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>229442.10526315792</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="C19" s="1"/>
+      <c r="H19" s="1">
+        <v>10.87058</v>
+      </c>
+      <c r="S19" s="3"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>239300.00000000003</v>
       </c>
+      <c r="C20" s="1"/>
+      <c r="H20" s="1">
+        <v>15.40395</v>
+      </c>
+      <c r="S20" s="3"/>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="H21" s="1">
+        <v>24.795680000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="H22" s="1">
+        <v>31.71949</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="H23" s="1">
+        <v>39.118980000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="H24" s="1">
+        <v>48.927660000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="H25" s="1">
+        <v>55.711190000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="H26" s="1">
+        <v>67.981570000000005</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F10"/>
+  <autoFilter ref="F1:F10" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386DBB15-2B7A-4B87-A827-3FE2F9E9A5BB}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>696.48140000000001</v>
+      </c>
+      <c r="D1" s="1">
+        <v>26.390930000000001</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4.2002480000000002</v>
+      </c>
+      <c r="F1" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1">
+        <v>696.48140000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2583.877</v>
+      </c>
+      <c r="D2" s="1">
+        <v>50.831850000000003</v>
+      </c>
+      <c r="E2" s="1">
+        <v>8.0901399999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2583.877</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4665.1480000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <v>68.30189</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10.87058</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4665.1480000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9367.5040000000008</v>
+      </c>
+      <c r="D4" s="1">
+        <v>96.78586</v>
+      </c>
+      <c r="E4" s="1">
+        <v>15.40395</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9367.5040000000008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>24272.34</v>
+      </c>
+      <c r="D5" s="1">
+        <v>155.79580000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>24.795680000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>24272.34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>39720.269999999997</v>
+      </c>
+      <c r="D6" s="1">
+        <v>199.29949999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>31.71949</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>39720.269999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>60413.62</v>
+      </c>
+      <c r="D7" s="1">
+        <v>245.79179999999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>39.118980000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>60413.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>94508</v>
+      </c>
+      <c r="D8" s="1">
+        <v>307.42149999999998</v>
+      </c>
+      <c r="E8" s="1">
+        <v>48.927660000000003</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>94508</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>122530.6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>350.0437</v>
+      </c>
+      <c r="E9" s="1">
+        <v>55.711190000000002</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>122530.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>182449.3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>427.14080000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>67.981570000000005</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>182449.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377519A5-2FCC-4EC4-ACCF-4A912F9793F9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>